<commit_message>
set github as mirror
</commit_message>
<xml_diff>
--- a/available_data.xlsx
+++ b/available_data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phl/thu-projects/label_gen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABF758A8-031E-0549-A73E-8D129BAC8E0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C05F1E3-5137-5542-B47E-E9B853BF3005}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="720" windowWidth="27480" windowHeight="16940" xr2:uid="{C7C155A9-EF16-5B45-89DD-05EA1BF03B01}"/>
+    <workbookView xWindow="5600" yWindow="3620" windowWidth="27480" windowHeight="14040" xr2:uid="{C7C155A9-EF16-5B45-89DD-05EA1BF03B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="available_data" localSheetId="0">Sheet1!$A$1:$F$18</definedName>
+    <definedName name="available_data" localSheetId="0">Sheet1!$A$1:$F$19</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DAE41A-4A77-484B-B8FE-B34A6E8DCA58}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,27 +714,27 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11">
-        <v>47236</v>
-      </c>
-      <c r="D11">
-        <v>101</v>
-      </c>
-      <c r="E11">
-        <v>3000</v>
-      </c>
-      <c r="F11">
-        <v>3000</v>
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -774,13 +774,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
       </c>
       <c r="C14">
-        <v>47229</v>
+        <v>47236</v>
       </c>
       <c r="D14">
         <v>101</v>
@@ -794,13 +794,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15">
-        <v>47235</v>
+        <v>47229</v>
       </c>
       <c r="D15">
         <v>101</v>
@@ -814,61 +814,81 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>294</v>
+        <v>47235</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="E16">
-        <v>1211</v>
+        <v>3000</v>
       </c>
       <c r="F16">
-        <v>1196</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C17">
-        <v>500</v>
+        <v>294</v>
       </c>
       <c r="D17">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>21519</v>
+        <v>1211</v>
       </c>
       <c r="F17">
-        <v>7077</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>500</v>
+      </c>
+      <c r="D18">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>21519</v>
+      </c>
+      <c r="F18">
+        <v>7077</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
         <v>103</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>14</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>1500</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>917</v>
       </c>
     </row>

</xml_diff>